<commit_message>
First commit of the data and script for testing my shape simulations on linear measurements of mandibles
</commit_message>
<xml_diff>
--- a/output/disp_results_summary.xlsx
+++ b/output/disp_results_summary.xlsx
@@ -155,21 +155,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,77 +473,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -567,22 +574,22 @@
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -608,22 +615,22 @@
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -643,28 +650,28 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="6" t="s">
+      <c r="H5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -675,7 +682,7 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
@@ -684,28 +691,28 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-ran all of the analyses with permutation tests of significance. Deleted the previous output files from rarefaction tests. New results summary in the excel file: tenrecs are not significantly more diverse than golden moles
</commit_message>
<xml_diff>
--- a/output/disp_results_summary.xlsx
+++ b/output/disp_results_summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>Data</t>
   </si>
@@ -42,9 +42,6 @@
     <t>T&gt;G*</t>
   </si>
   <si>
-    <t>lower*</t>
-  </si>
-  <si>
     <t>Skulls ventral</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>ProdRange</t>
+  </si>
+  <si>
+    <t>Mandibles one curve</t>
   </si>
 </sst>
 </file>
@@ -96,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +106,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -170,6 +176,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,12 +482,12 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.21875" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
@@ -492,19 +500,19 @@
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
@@ -513,16 +521,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>3</v>
@@ -563,17 +571,15 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
@@ -589,73 +595,65 @@
       <c r="L3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="L4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="3" t="s">
         <v>6</v>
       </c>
@@ -671,54 +669,80 @@
       <c r="L5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="G7" s="1"/>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Completed drafts of disparity paper and supplementary, ready for comments from Natalie
</commit_message>
<xml_diff>
--- a/output/disp_results_summary.xlsx
+++ b/output/disp_results_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="18180" windowHeight="9264"/>
+    <workbookView xWindow="480" yWindow="156" windowWidth="18180" windowHeight="9204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,6 +167,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,8 +178,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,22 +543,22 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="9" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -617,19 +617,19 @@
         <v>10</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="3"/>
@@ -681,7 +681,7 @@
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -724,7 +724,7 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="1"/>

</xml_diff>